<commit_message>
init data & make sign in/up UI
</commit_message>
<xml_diff>
--- a/scrapeData/suppilers.xlsx
+++ b/scrapeData/suppilers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\GMH\scrapeData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE1849B-740D-49DF-88A3-18B659A38D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A08F67-FC56-4141-BBB1-F6BCAD097667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F9FBF81D-81BF-4EDE-AF2C-5CB62DA5C78B}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>STT</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -435,21 +432,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6298BA41-6FAD-48E8-BEF7-B3725C694A6C}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="50.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="51.7109375" customWidth="1"/>
+    <col min="3" max="3" width="109.85546875" customWidth="1"/>
     <col min="4" max="4" width="113.42578125" customWidth="1"/>
     <col min="5" max="5" width="100.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,92 +457,71 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>128317</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>128317</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>225160</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>225160</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>256763</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>256763</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>74087</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>74087</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>123782</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>123782</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>203678</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>203678</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>